<commit_message>
Auto-committed on 2022/05/12 週四
</commit_message>
<xml_diff>
--- a/Program/Other/L9731_底稿_人工檢核表1.xlsx
+++ b/Program/Other/L9731_底稿_人工檢核表1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>戶號</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -58,6 +58,10 @@
   </si>
   <si>
     <t>資產分類</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>不足額金額</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1047,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1063,9 +1067,10 @@
     <col min="6" max="6" width="18.453125" style="2" customWidth="1"/>
     <col min="7" max="7" width="7.90625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1091,6 +1096,9 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/08/25 週五 11:47:53.35
</commit_message>
<xml_diff>
--- a/Program/Other/L9731_底稿_人工檢核表1.xlsx
+++ b/Program/Other/L9731_底稿_人工檢核表1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yah12\Desktop\重要\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE9A66C-3C14-46BF-AB9E-02F2135F7299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="五類資產檢核表" sheetId="3" r:id="rId1"/>
@@ -17,21 +18,12 @@
   <definedNames>
     <definedName name="_xlnm.Database">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>戶號</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -61,14 +53,18 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>不足額金額</t>
+    <t>無擔保金額</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>無擔保資產分類</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -722,11 +718,11 @@
     <cellStyle name="60% - 輔色5" xfId="17" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - 輔色6" xfId="18" builtinId="52" customBuiltin="1"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="19"/>
-    <cellStyle name="一般 3 2" xfId="20"/>
+    <cellStyle name="一般 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="一般 3 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="千分位" xfId="21" builtinId="3"/>
-    <cellStyle name="千分位 2" xfId="22"/>
-    <cellStyle name="千分位 3" xfId="23"/>
+    <cellStyle name="千分位 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="千分位 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="中等" xfId="24" builtinId="28" customBuiltin="1"/>
     <cellStyle name="合計" xfId="25" builtinId="25" customBuiltin="1"/>
     <cellStyle name="好" xfId="26" builtinId="26" customBuiltin="1"/>
@@ -765,9 +761,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -805,9 +801,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -842,7 +838,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -877,7 +873,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1050,27 +1046,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1099,6 +1096,9 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/08/25 週五 16:51:47.44
</commit_message>
<xml_diff>
--- a/Program/Other/L9731_底稿_人工檢核表1.xlsx
+++ b/Program/Other/L9731_底稿_人工檢核表1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yah12\Desktop\重要\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE9A66C-3C14-46BF-AB9E-02F2135F7299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C316BE54-770A-43F7-B389-8C4C66237A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,15 +49,15 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>資產分類</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>無擔保金額</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
     <t>無擔保資產分類</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>資產分類2</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1062,7 +1062,7 @@
     <col min="5" max="5" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="7.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1091,13 +1091,13 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>